<commit_message>
- updated Test cases for Correlation for Lk
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B46FA-4F40-4D2D-854F-60C7AAEA2128}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF81FC7-99B7-4259-B563-549D5C6B6178}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="128">
   <si>
     <t>S/N</t>
   </si>
@@ -425,29 +424,125 @@
  form of scatterplot diagram</t>
   </si>
   <si>
-    <t>inventory_data_sample_masked &amp;
-movement_data_sample_masked  database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Login.
-2. Choose inventory_data_sample_masked &amp; movement_data_sample_masked databse from correlation's chart view
-3. Choose Inventory and OrderQuantity to be shown in chart
+    <t>Chart shown with min/max value</t>
+  </si>
+  <si>
+    <t>Upload failed without error message</t>
+  </si>
+  <si>
+    <t>Export failed</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Chart is not shown upon request</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> weather_data_2017_3_months &amp;
+movement_data_sample_masked  data set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by geographicallocation and value Singapore
 </t>
   </si>
   <si>
-    <t>Chart shown with min/max value</t>
-  </si>
-  <si>
-    <t>Upload failed without error message</t>
-  </si>
-  <si>
-    <t>Export failed</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Chart is not shown upon request</t>
+    <t>Visualise two types of data in the
+ form of scatterplot diagram (validations in data sets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Dont select filter
+6. Generate Scatterplot
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by date or activitydate and range between 01/01/2017 to 01/02/2017
+6. Generate Scatterplot
+</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by company and value DHL
+6. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by depot and value 34
+6. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t>Error Validations shown</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose don’t select data set 2
+3. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose don’t select data set 1
+3. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose don’t select variable X
+3. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose don’t select variable Y
+3. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by date or activitydate and don't select range 
+6. Generate Scatterplot
+</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by company and don't select company value
+6. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t>1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by depot and don't select depot value
+6. Generate Scatterplot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login and select correlation tab
+2. Choose weather_data_2017_3_months &amp; movement_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on activity date
+4. Choose Inventory as X variable and OrderQuantity as Y variable to be shown in chart
+5. Select filter by geographicallocation and don't select geographicallocation value
+</t>
   </si>
 </sst>
 </file>
@@ -653,6 +748,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,10 +762,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -675,34 +780,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -710,20 +805,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -735,10 +830,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1030,33 +1125,33 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.47265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.05078125" customWidth="1"/>
-    <col min="5" max="5" width="50.83984375" customWidth="1"/>
-    <col min="6" max="6" width="40.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.47265625" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="50.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -1068,13 +1163,13 @@
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1088,20 +1183,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
+    <row r="3" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>47</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -1110,40 +1205,40 @@
       <c r="G3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="18"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" ht="21.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="H4" s="17"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" ht="21.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="13" t="s">
         <v>58</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1152,14 +1247,14 @@
       <c r="G5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+      <c r="H5" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
@@ -1168,24 +1263,24 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
+      <c r="H6" s="25"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1194,14 +1289,14 @@
       <c r="G7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
+      <c r="H7" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
@@ -1210,24 +1305,24 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
+      <c r="H8" s="25"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="13" t="s">
         <v>60</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -1236,14 +1331,14 @@
       <c r="G9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="9"/>
+    <row r="10" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
@@ -1252,24 +1347,24 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8">
+    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="13" t="s">
         <v>88</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1278,14 +1373,14 @@
       <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1" t="s">
@@ -1294,24 +1389,24 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8">
+    <row r="13" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>4</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="13" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1320,14 +1415,14 @@
       <c r="G13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="9"/>
+      <c r="H13" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="1" t="s">
@@ -1336,24 +1431,24 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8">
+      <c r="H14" s="25"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
         <v>5</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="13" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -1362,14 +1457,14 @@
       <c r="G15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="9"/>
+      <c r="H15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1" t="s">
@@ -1378,24 +1473,24 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="8">
+      <c r="H16" s="25"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <v>6</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="12" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="13" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1404,14 +1499,14 @@
       <c r="G17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="9"/>
+      <c r="H17" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1" t="s">
@@ -1420,12 +1515,72 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="17"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A9:A10"/>
@@ -1442,66 +1597,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1515,45 +1610,45 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.3671875" customWidth="1"/>
-    <col min="5" max="5" width="62.05078125" customWidth="1"/>
-    <col min="6" max="6" width="39.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.9453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.47265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.9453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.47265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.9453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.47265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.9453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.47265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.9453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.47265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.9453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="6" max="6" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -1565,13 +1660,13 @@
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="1:11" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1585,20 +1680,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
+    <row r="3" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -1607,18 +1702,18 @@
       <c r="G3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+      <c r="J3" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
@@ -1627,24 +1722,24 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1653,18 +1748,18 @@
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+      <c r="J5" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
@@ -1673,24 +1768,24 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1699,18 +1794,18 @@
       <c r="G7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
+      <c r="J7" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
@@ -1719,24 +1814,24 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="13"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -1745,44 +1840,44 @@
       <c r="G9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="9"/>
+      <c r="J9" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="13"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8">
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1791,21 +1886,21 @@
       <c r="G11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="9"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1" t="s">
@@ -1814,24 +1909,24 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8">
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1840,18 +1935,18 @@
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="9"/>
+      <c r="J13" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="1" t="s">
@@ -1860,24 +1955,24 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8">
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
         <v>7</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -1888,8 +1983,8 @@
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1" t="s">
@@ -1902,32 +1997,32 @@
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
     </row>
-    <row r="17" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="8">
+    <row r="17" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <v>8</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="12" t="s">
         <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="9"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1" t="s">
@@ -1935,25 +2030,25 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="8">
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
         <v>9</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -1964,8 +2059,8 @@
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="9"/>
+    <row r="20" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="1" t="s">
@@ -1980,15 +2075,70 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
@@ -2005,70 +2155,15 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2078,35 +2173,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F238631-EBC5-4720-B916-747C7C12E944}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:AF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.41796875" customWidth="1"/>
-    <col min="3" max="3" width="20.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.3671875" customWidth="1"/>
-    <col min="5" max="5" width="32.89453125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -2118,13 +2213,13 @@
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2138,20 +2233,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>75</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -2160,42 +2255,42 @@
       <c r="G3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="30"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="G4" s="11"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="13" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -2204,42 +2299,42 @@
       <c r="G5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="16" t="s">
         <v>89</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
+      <c r="G6" s="11"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>75</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -2248,130 +2343,132 @@
       <c r="G7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="16" t="s">
         <v>89</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
+      <c r="G8" s="11"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="13" t="s">
         <v>75</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="32"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="9"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8">
+      <c r="G10" s="19"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="13" t="s">
         <v>75</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="32"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="J11" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="48.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:10" ht="48.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -2388,28 +2485,26 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2420,33 +2515,33 @@
   <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:T10"/>
+      <selection activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.3671875" customWidth="1"/>
-    <col min="5" max="5" width="40.68359375" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -2502,13 +2597,13 @@
       </c>
       <c r="AF1" s="21"/>
     </row>
-    <row r="2" spans="1:32" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="1:32" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2588,20 +2683,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
+    <row r="3" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>82</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -2610,106 +2705,106 @@
       <c r="G3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J3" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P3" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="U3" s="6"/>
-      <c r="V3" s="29"/>
+      <c r="V3" s="32"/>
       <c r="W3" s="6"/>
-      <c r="X3" s="29"/>
+      <c r="X3" s="32"/>
       <c r="Y3" s="6"/>
-      <c r="Z3" s="29"/>
+      <c r="Z3" s="32"/>
       <c r="AA3" s="6"/>
-      <c r="AB3" s="29"/>
+      <c r="AB3" s="32"/>
       <c r="AC3" s="6"/>
-      <c r="AD3" s="29"/>
+      <c r="AD3" s="32"/>
       <c r="AE3" s="6"/>
-      <c r="AF3" s="29"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+      <c r="AF3" s="32"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="30"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="11"/>
       <c r="J4" s="34"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="9"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="11"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="13"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="7"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-    </row>
-    <row r="5" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="T4" s="25"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+    </row>
+    <row r="5" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="13" t="s">
         <v>83</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -2718,106 +2813,106 @@
       <c r="G5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>89</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P5" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="16" t="s">
         <v>89</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="6"/>
-      <c r="V5" s="29"/>
+      <c r="V5" s="32"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="29"/>
+      <c r="X5" s="32"/>
       <c r="Y5" s="6"/>
-      <c r="Z5" s="29"/>
+      <c r="Z5" s="32"/>
       <c r="AA5" s="6"/>
-      <c r="AB5" s="29"/>
+      <c r="AB5" s="32"/>
       <c r="AC5" s="6"/>
-      <c r="AD5" s="29"/>
+      <c r="AD5" s="32"/>
       <c r="AE5" s="6"/>
-      <c r="AF5" s="29"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+      <c r="AF5" s="32"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="34"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="13"/>
+      <c r="L6" s="25"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="9"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="11"/>
       <c r="P6" s="34"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="13"/>
+      <c r="R6" s="25"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-    </row>
-    <row r="7" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
+      <c r="T6" s="25"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+    </row>
+    <row r="7" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>84</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -2826,230 +2921,289 @@
       <c r="G7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J7" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>89</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P7" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P7" s="16" t="s">
         <v>89</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="T7" s="12" t="s">
+      <c r="T7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="U7" s="6"/>
-      <c r="V7" s="29"/>
+      <c r="V7" s="32"/>
       <c r="W7" s="6"/>
-      <c r="X7" s="29"/>
+      <c r="X7" s="32"/>
       <c r="Y7" s="6"/>
-      <c r="Z7" s="29"/>
+      <c r="Z7" s="32"/>
       <c r="AA7" s="6"/>
-      <c r="AB7" s="29"/>
+      <c r="AB7" s="32"/>
       <c r="AC7" s="6"/>
-      <c r="AD7" s="29"/>
+      <c r="AD7" s="32"/>
       <c r="AE7" s="6"/>
-      <c r="AF7" s="29"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
+      <c r="AF7" s="32"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="34"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="13"/>
+      <c r="L8" s="25"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="9"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="11"/>
       <c r="P8" s="34"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="13"/>
+      <c r="R8" s="25"/>
       <c r="S8" s="7"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-    </row>
-    <row r="9" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
+      <c r="T8" s="25"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+    </row>
+    <row r="9" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="13" t="s">
         <v>84</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="36"/>
       <c r="I9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J9" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>89</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="N9" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P9" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P9" s="16" t="s">
         <v>89</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="R9" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="24" t="s">
         <v>86</v>
       </c>
       <c r="U9" s="6"/>
-      <c r="V9" s="29"/>
+      <c r="V9" s="32"/>
       <c r="W9" s="6"/>
-      <c r="X9" s="29"/>
+      <c r="X9" s="32"/>
       <c r="Y9" s="6"/>
-      <c r="Z9" s="29"/>
+      <c r="Z9" s="32"/>
       <c r="AA9" s="6"/>
-      <c r="AB9" s="29"/>
+      <c r="AB9" s="32"/>
       <c r="AC9" s="6"/>
-      <c r="AD9" s="29"/>
+      <c r="AD9" s="32"/>
       <c r="AE9" s="6"/>
-      <c r="AF9" s="29"/>
-    </row>
-    <row r="10" spans="1:32" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="9"/>
+      <c r="AF9" s="32"/>
+    </row>
+    <row r="10" spans="1:32" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="35"/>
       <c r="H10" s="37"/>
-      <c r="I10" s="9"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="34"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="13"/>
+      <c r="L10" s="25"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="9"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="11"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="7"/>
-      <c r="R10" s="13"/>
+      <c r="R10" s="25"/>
       <c r="S10" s="7"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="147">
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="O1:P1"/>
@@ -3074,97 +3228,38 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB5:AB6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3178,32 +3273,32 @@
       <selection activeCell="Q3" sqref="Q3:R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.47265625" customWidth="1"/>
-    <col min="3" max="3" width="32.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.3671875" customWidth="1"/>
-    <col min="5" max="5" width="40.68359375" customWidth="1"/>
-    <col min="6" max="6" width="10.734375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:30" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -3255,13 +3350,13 @@
       </c>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:30" ht="39.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="1:30" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3335,20 +3430,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8">
+    <row r="3" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -3357,98 +3452,98 @@
       <c r="G3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S3" s="6"/>
-      <c r="T3" s="29"/>
+      <c r="T3" s="32"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="29"/>
+      <c r="V3" s="32"/>
       <c r="W3" s="6"/>
-      <c r="X3" s="29"/>
+      <c r="X3" s="32"/>
       <c r="Y3" s="6"/>
-      <c r="Z3" s="29"/>
+      <c r="Z3" s="32"/>
       <c r="AA3" s="6"/>
-      <c r="AB3" s="29"/>
+      <c r="AB3" s="32"/>
       <c r="AC3" s="6"/>
-      <c r="AD3" s="29"/>
-    </row>
-    <row r="4" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+      <c r="AD3" s="32"/>
+    </row>
+    <row r="4" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="13"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="13"/>
+      <c r="N4" s="25"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="13"/>
+      <c r="P4" s="25"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-    </row>
-    <row r="5" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
+      <c r="R4" s="25"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+    </row>
+    <row r="5" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="13" t="s">
         <v>103</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -3457,98 +3552,98 @@
       <c r="G5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S5" s="6"/>
-      <c r="T5" s="29"/>
+      <c r="T5" s="32"/>
       <c r="U5" s="6"/>
-      <c r="V5" s="29"/>
+      <c r="V5" s="32"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="29"/>
+      <c r="X5" s="32"/>
       <c r="Y5" s="6"/>
-      <c r="Z5" s="29"/>
+      <c r="Z5" s="32"/>
       <c r="AA5" s="6"/>
-      <c r="AB5" s="29"/>
+      <c r="AB5" s="32"/>
       <c r="AC5" s="6"/>
-      <c r="AD5" s="29"/>
-    </row>
-    <row r="6" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+      <c r="AD5" s="32"/>
+    </row>
+    <row r="6" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="25"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="13"/>
+      <c r="L6" s="25"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="13"/>
+      <c r="N6" s="25"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="13"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-    </row>
-    <row r="7" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
+      <c r="R6" s="25"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+    </row>
+    <row r="7" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>103</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -3557,112 +3652,144 @@
       <c r="G7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="P7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="24" t="s">
         <v>86</v>
       </c>
       <c r="S7" s="6"/>
-      <c r="T7" s="29"/>
+      <c r="T7" s="32"/>
       <c r="U7" s="6"/>
-      <c r="V7" s="29"/>
+      <c r="V7" s="32"/>
       <c r="W7" s="6"/>
-      <c r="X7" s="29"/>
+      <c r="X7" s="32"/>
       <c r="Y7" s="6"/>
-      <c r="Z7" s="29"/>
+      <c r="Z7" s="32"/>
       <c r="AA7" s="6"/>
-      <c r="AB7" s="29"/>
+      <c r="AB7" s="32"/>
       <c r="AC7" s="6"/>
-      <c r="AD7" s="29"/>
-    </row>
-    <row r="8" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
+      <c r="AD7" s="32"/>
+    </row>
+    <row r="8" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="13"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="13"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="13"/>
+      <c r="L8" s="25"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="13"/>
+      <c r="N8" s="25"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="13"/>
+      <c r="P8" s="25"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="Z3:Z4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
@@ -3687,64 +3814,32 @@
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="S5:S6"/>
     <mergeCell ref="T5:T6"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="W7:W8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3752,36 +3847,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A32C82-4E28-47DA-B010-C23DCFFA9445}">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.3671875" customWidth="1"/>
-    <col min="5" max="5" width="40.68359375" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -3829,13 +3924,13 @@
       </c>
       <c r="AB1" s="21"/>
     </row>
-    <row r="2" spans="1:28" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="1:28" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3903,8 +3998,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="3" customFormat="1" ht="45.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="38">
+    <row r="3" spans="1:28" s="3" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39">
         <v>1</v>
       </c>
       <c r="B3" s="40" t="s">
@@ -3914,42 +4009,42 @@
         <v>106</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H3" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>86</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="N3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="P3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="Q3" s="6"/>
@@ -3965,60 +4060,487 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row r="4" spans="1:28" s="3" customFormat="1" ht="45.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="39"/>
+    <row r="4" spans="1:28" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="34"/>
-      <c r="K4" s="39"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="34"/>
-      <c r="M4" s="39"/>
+      <c r="M4" s="38"/>
       <c r="N4" s="34"/>
-      <c r="O4" s="39"/>
+      <c r="O4" s="38"/>
       <c r="P4" s="34"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="39"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+    </row>
+    <row r="5" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39">
+        <v>2</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+    </row>
+    <row r="7" spans="1:28" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
+        <v>3</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:28" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
+        <v>4</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:28" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39">
+        <v>5</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
+        <v>6</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="39">
+        <v>7</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="39">
+        <v>8</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="39">
+        <v>9</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="39">
+        <v>10</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39">
+        <v>11</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+    </row>
+    <row r="25" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="39">
+        <v>12</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+    </row>
+    <row r="27" spans="1:6" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="39">
+        <v>13</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+    </row>
+    <row r="29" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="39">
+        <v>14</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
+  <mergeCells count="123">
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -4035,13 +4557,28 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update view datasets in test cases
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF81FC7-99B7-4259-B563-549D5C6B6178}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{AAF81FC7-99B7-4259-B563-549D5C6B6178}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FEF09AD7-F6B6-4E8C-A412-DB908D08E04D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="133">
   <si>
     <t>S/N</t>
   </si>
@@ -544,12 +544,30 @@
 5. Select filter by geographicallocation and don't select geographicallocation value
 </t>
   </si>
+  <si>
+    <t>View Datasets</t>
+  </si>
+  <si>
+    <t>Save the combined table from two tables using a common variable</t>
+  </si>
+  <si>
+    <t>inventory_data_sample_masked &amp; skudetails_data_sample_masked</t>
+  </si>
+  <si>
+    <t>1. Login and select View Datasets tab
+2. Choose inventory_data_sample_masked &amp; skudetails_data_sample_masked as data set 1 and data set 2 respectively
+3. Choose to combine based on Depot
+4. Click button to combine datasets &amp; save</t>
+  </si>
+  <si>
+    <t>A combined table is shown</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +621,18 @@
       <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -727,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -744,50 +774,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -797,7 +789,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -805,20 +835,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -838,6 +868,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,33 +1166,33 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="50.88671875" customWidth="1"/>
-    <col min="6" max="6" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="50.86328125" customWidth="1"/>
+    <col min="6" max="6" width="40.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -1163,13 +1204,13 @@
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1183,78 +1224,78 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:10" ht="29.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="17"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="23"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" ht="21.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="H4" s="20"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" ht="21.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="26"/>
-    </row>
-    <row r="6" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="H5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
@@ -1263,40 +1304,40 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="26"/>
-    </row>
-    <row r="8" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="H7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
@@ -1305,40 +1346,40 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="H8" s="11"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="16">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="10" t="s">
         <v>86</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="17"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
@@ -1347,40 +1388,40 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="25"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="16">
         <v>3</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="10" t="s">
         <v>86</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="17"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1" t="s">
@@ -1389,40 +1430,40 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="25"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+    <row r="13" spans="1:10" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="16">
         <v>4</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="26"/>
-    </row>
-    <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
+      <c r="H13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="17"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="1" t="s">
@@ -1431,40 +1472,40 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="16">
         <v>5</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="26"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="H15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="17"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1" t="s">
@@ -1473,40 +1514,40 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="H16" s="11"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="16">
         <v>6</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="H17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="17"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1" t="s">
@@ -1515,24 +1556,60 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="J13:J14"/>
@@ -1549,54 +1626,18 @@
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1610,45 +1651,45 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
-    <col min="6" max="6" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.46484375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.46484375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.46484375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.46484375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.46484375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -1660,13 +1701,13 @@
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:11" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1680,40 +1721,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="J3" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="17"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
@@ -1722,44 +1763,44 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="25"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="J5" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
@@ -1768,44 +1809,44 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="25"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="J7" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
@@ -1814,93 +1855,93 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="16">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="J9" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="17"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="25"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="16">
         <v>5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="10" t="s">
         <v>86</v>
       </c>
       <c r="K11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="17"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1" t="s">
@@ -1909,44 +1950,44 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="25"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="25"/>
-    </row>
-    <row r="13" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="16">
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
+      <c r="J13" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="17"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="1" t="s">
@@ -1955,27 +1996,27 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="25"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="25"/>
-    </row>
-    <row r="15" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="27"/>
@@ -1983,8 +2024,8 @@
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+    <row r="16" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="17"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1" t="s">
@@ -1997,32 +2038,32 @@
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
     </row>
-    <row r="17" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+    <row r="17" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="16">
         <v>8</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="17"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1" t="s">
@@ -2030,28 +2071,28 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-    </row>
-    <row r="19" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="16">
         <v>9</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="27"/>
@@ -2059,8 +2100,8 @@
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="17"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="1" t="s">
@@ -2075,54 +2116,31 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="G13:G14"/>
@@ -2139,31 +2157,54 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2177,31 +2218,31 @@
       <selection activeCell="K1" sqref="K1:AF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" customWidth="1"/>
+    <col min="3" max="3" width="20.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="32.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -2213,13 +2254,13 @@
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2233,242 +2274,240 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="17"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="33"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="G4" s="17"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="33"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="G6" s="17"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="33"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="G8" s="17"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="16">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="6" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="17"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="33"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="G10" s="13"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="16">
         <v>5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="6" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="48.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:10" ht="48.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="17"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="33"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="17"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -2485,26 +2524,28 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2518,30 +2559,30 @@
       <selection activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -2597,13 +2638,13 @@
       </c>
       <c r="AF1" s="21"/>
     </row>
-    <row r="2" spans="1:32" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:32" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2683,456 +2724,539 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="6" t="s">
+      <c r="N3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="R3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S3" s="6" t="s">
+      <c r="R3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="T3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="U3" s="6"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="32"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="T3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="U3" s="9"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="29"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A4" s="17"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="33"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="34"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="25"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="17"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="25"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="7"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-    </row>
-    <row r="5" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="T4" s="11"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+    </row>
+    <row r="5" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M5" s="6" t="s">
+      <c r="L5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="6" t="s">
+      <c r="N5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S5" s="6" t="s">
+      <c r="R5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="T5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="32"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="T5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" s="9"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="29"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="33"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="34"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="25"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="17"/>
       <c r="P6" s="34"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="25"/>
+      <c r="R6" s="11"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-    </row>
-    <row r="7" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="T6" s="11"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+    </row>
+    <row r="7" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M7" s="6" t="s">
+      <c r="L7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O7" s="6" t="s">
+      <c r="N7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="R7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S7" s="6" t="s">
+      <c r="R7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="T7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="U7" s="6"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="32"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="32"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="32"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="T7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" s="9"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="29"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="33"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="34"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="25"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="17"/>
       <c r="P8" s="34"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="25"/>
+      <c r="R8" s="11"/>
       <c r="S8" s="7"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-    </row>
-    <row r="9" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="T8" s="11"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+    </row>
+    <row r="9" spans="1:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="16">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="36"/>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M9" s="6" t="s">
+      <c r="L9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O9" s="6" t="s">
+      <c r="N9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="R9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S9" s="6" t="s">
+      <c r="R9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="T9" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="U9" s="6"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="32"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="32"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="32"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="32"/>
-    </row>
-    <row r="10" spans="1:32" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="T9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="U9" s="9"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="29"/>
+    </row>
+    <row r="10" spans="1:32" ht="21.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="17"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="33"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="35"/>
       <c r="H10" s="37"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="34"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="25"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="17"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="7"/>
-      <c r="R10" s="25"/>
+      <c r="R10" s="11"/>
       <c r="S10" s="7"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="147">
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
     <mergeCell ref="AF5:AF6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -3157,109 +3281,26 @@
     <mergeCell ref="X5:X6"/>
     <mergeCell ref="Y5:Y6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3273,32 +3314,32 @@
       <selection activeCell="Q3" sqref="Q3:R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.46484375" customWidth="1"/>
+    <col min="3" max="3" width="32.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:30" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -3350,13 +3391,13 @@
       </c>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:30" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:30" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3430,308 +3471,392 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="6" t="s">
+      <c r="N3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="P3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q3" s="6" t="s">
+      <c r="P3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="32"/>
-    </row>
-    <row r="4" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="R3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" s="9"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="29"/>
+    </row>
+    <row r="4" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="17"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="25"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="25"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="25"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="25"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="25"/>
+      <c r="P4" s="11"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-    </row>
-    <row r="5" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="R4" s="11"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+    </row>
+    <row r="5" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M5" s="6" t="s">
+      <c r="L5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="N5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="6" t="s">
+      <c r="N5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q5" s="6" t="s">
+      <c r="P5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="R5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="32"/>
-    </row>
-    <row r="6" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="R5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S5" s="9"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="29"/>
+    </row>
+    <row r="6" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="25"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="25"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="25"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="25"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="25"/>
+      <c r="P6" s="11"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-    </row>
-    <row r="7" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="R6" s="11"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+    </row>
+    <row r="7" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" s="6" t="s">
+      <c r="J7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="L7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M7" s="6" t="s">
+      <c r="L7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="N7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="O7" s="6" t="s">
+      <c r="N7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="P7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q7" s="6" t="s">
+      <c r="P7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="R7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S7" s="6"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="32"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="32"/>
-    </row>
-    <row r="8" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="R7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S7" s="9"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="29"/>
+    </row>
+    <row r="8" spans="1:30" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="25"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="25"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="25"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="25"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="AC1:AD1"/>
@@ -3756,90 +3881,6 @@
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="AB5:AB6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3847,36 +3888,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A32C82-4E28-47DA-B010-C23DCFFA9445}">
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -3924,13 +3965,13 @@
       </c>
       <c r="AB1" s="21"/>
     </row>
-    <row r="2" spans="1:28" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:28" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3998,7 +4039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="3" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="3" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="39">
         <v>1</v>
       </c>
@@ -4008,67 +4049,67 @@
       <c r="C3" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-    </row>
-    <row r="4" spans="1:28" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+    </row>
+    <row r="4" spans="1:28" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="38"/>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
-      <c r="D4" s="23"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
-      <c r="H4" s="25"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="38"/>
       <c r="J4" s="34"/>
       <c r="K4" s="38"/>
@@ -4090,7 +4131,7 @@
       <c r="AA4" s="38"/>
       <c r="AB4" s="38"/>
     </row>
-    <row r="5" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="39">
         <v>2</v>
       </c>
@@ -4100,25 +4141,25 @@
       <c r="C5" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="79.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="38"/>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
-      <c r="D6" s="23"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
     </row>
-    <row r="7" spans="1:28" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="39">
         <v>3</v>
       </c>
@@ -4128,25 +4169,25 @@
       <c r="C7" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="102.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
-      <c r="D8" s="23"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
     </row>
-    <row r="9" spans="1:28" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="71.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="39">
         <v>4</v>
       </c>
@@ -4156,25 +4197,25 @@
       <c r="C9" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="52.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
-      <c r="D10" s="23"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
     </row>
-    <row r="11" spans="1:28" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="42.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="39">
         <v>5</v>
       </c>
@@ -4184,25 +4225,25 @@
       <c r="C11" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="91.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
-      <c r="D12" s="23"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A13" s="39">
         <v>6</v>
       </c>
@@ -4212,25 +4253,25 @@
       <c r="C13" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="88.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
-      <c r="D14" s="23"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
     </row>
-    <row r="15" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="39">
         <v>7</v>
       </c>
@@ -4240,25 +4281,25 @@
       <c r="C15" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="58.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
-      <c r="D16" s="23"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="38"/>
       <c r="F16" s="38"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="39">
         <v>8</v>
       </c>
@@ -4268,25 +4309,25 @@
       <c r="C17" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
-      <c r="D18" s="23"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="38"/>
       <c r="F18" s="38"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="39">
         <v>9</v>
       </c>
@@ -4296,25 +4337,25 @@
       <c r="C19" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
-      <c r="D20" s="23"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="39">
         <v>10</v>
       </c>
@@ -4324,25 +4365,25 @@
       <c r="C21" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
-      <c r="D22" s="23"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="38"/>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="39">
         <v>11</v>
       </c>
@@ -4352,25 +4393,25 @@
       <c r="C23" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="99.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="38"/>
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
-      <c r="D24" s="23"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
     </row>
-    <row r="25" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="39">
         <v>12</v>
       </c>
@@ -4380,25 +4421,25 @@
       <c r="C25" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="38"/>
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
-      <c r="D26" s="23"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="38"/>
       <c r="F26" s="38"/>
     </row>
-    <row r="27" spans="1:6" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="58.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="39">
         <v>13</v>
       </c>
@@ -4408,25 +4449,25 @@
       <c r="C27" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="104.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
-      <c r="D28" s="23"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
     </row>
-    <row r="29" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="39">
         <v>14</v>
       </c>
@@ -4436,104 +4477,67 @@
       <c r="C29" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+    <row r="30" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+    </row>
+    <row r="31" spans="1:6" ht="77.25" x14ac:dyDescent="0.45">
+      <c r="A31" s="43">
+        <v>15</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="123">
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4558,28 +4562,86 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>